<commit_message>
Added Lithium Ion Polymer Battery to components list
</commit_message>
<xml_diff>
--- a/FAIO_BOM.xlsx
+++ b/FAIO_BOM.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="65">
   <si>
     <t>Index</t>
   </si>
@@ -202,6 +202,18 @@
   </si>
   <si>
     <t>Total Price (CAD)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">All </t>
+  </si>
+  <si>
+    <t>PRT-13851</t>
+  </si>
+  <si>
+    <t xml:space="preserve">BATTERY LITHIUM 3.7V 400MAH </t>
+  </si>
+  <si>
+    <t xml:space="preserve">1568-1493-ND </t>
   </si>
 </sst>
 </file>
@@ -558,10 +570,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:J19"/>
+  <dimension ref="A1:J20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L6" sqref="L6"/>
+      <selection activeCell="E23" sqref="E23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -928,42 +940,35 @@
       <c r="I12">
         <v>40.200000000000003</v>
       </c>
-      <c r="J12">
-        <f>SUM(I2:I12)</f>
-        <v>57.028999999999996</v>
-      </c>
     </row>
     <row r="13" spans="1:10">
       <c r="A13">
         <v>12</v>
       </c>
       <c r="B13" t="s">
-        <v>54</v>
+        <v>61</v>
       </c>
       <c r="C13">
         <v>1</v>
       </c>
       <c r="D13" t="s">
-        <v>37</v>
+        <v>64</v>
       </c>
       <c r="E13" t="s">
-        <v>38</v>
+        <v>62</v>
       </c>
       <c r="F13" t="s">
-        <v>39</v>
-      </c>
-      <c r="G13" t="s">
-        <v>10</v>
+        <v>63</v>
       </c>
       <c r="H13">
         <v>0</v>
       </c>
       <c r="I13">
-        <v>14.33</v>
+        <v>6.17</v>
       </c>
       <c r="J13">
         <f>SUM(I2:I13)</f>
-        <v>71.358999999999995</v>
+        <v>63.198999999999998</v>
       </c>
     </row>
     <row r="14" spans="1:10">
@@ -971,19 +976,19 @@
         <v>13</v>
       </c>
       <c r="B14" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="C14">
         <v>1</v>
       </c>
       <c r="D14" t="s">
-        <v>34</v>
-      </c>
-      <c r="E14">
-        <v>110990027</v>
+        <v>37</v>
+      </c>
+      <c r="E14" t="s">
+        <v>38</v>
       </c>
       <c r="F14" t="s">
-        <v>35</v>
+        <v>39</v>
       </c>
       <c r="G14" t="s">
         <v>10</v>
@@ -992,7 +997,11 @@
         <v>0</v>
       </c>
       <c r="I14">
-        <v>3.97</v>
+        <v>14.33</v>
+      </c>
+      <c r="J14">
+        <f>SUM(I2:I14)</f>
+        <v>77.528999999999996</v>
       </c>
     </row>
     <row r="15" spans="1:10">
@@ -1000,19 +1009,19 @@
         <v>14</v>
       </c>
       <c r="B15" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="C15">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="D15" t="s">
-        <v>7</v>
-      </c>
-      <c r="E15" t="s">
-        <v>8</v>
+        <v>34</v>
+      </c>
+      <c r="E15">
+        <v>110990027</v>
       </c>
       <c r="F15" t="s">
-        <v>9</v>
+        <v>35</v>
       </c>
       <c r="G15" t="s">
         <v>10</v>
@@ -1021,7 +1030,7 @@
         <v>0</v>
       </c>
       <c r="I15">
-        <v>0.16</v>
+        <v>3.97</v>
       </c>
     </row>
     <row r="16" spans="1:10">
@@ -1032,16 +1041,16 @@
         <v>56</v>
       </c>
       <c r="C16">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="D16" t="s">
-        <v>28</v>
-      </c>
-      <c r="E16">
-        <v>4808</v>
+        <v>7</v>
+      </c>
+      <c r="E16" t="s">
+        <v>8</v>
       </c>
       <c r="F16" t="s">
-        <v>29</v>
+        <v>9</v>
       </c>
       <c r="G16" t="s">
         <v>10</v>
@@ -1050,7 +1059,7 @@
         <v>0</v>
       </c>
       <c r="I16">
-        <v>0.71699999999999997</v>
+        <v>0.16</v>
       </c>
     </row>
     <row r="17" spans="1:10">
@@ -1064,13 +1073,13 @@
         <v>4</v>
       </c>
       <c r="D17" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="E17">
-        <v>9605</v>
+        <v>4808</v>
       </c>
       <c r="F17" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="G17" t="s">
         <v>10</v>
@@ -1079,7 +1088,7 @@
         <v>0</v>
       </c>
       <c r="I17">
-        <v>0.248</v>
+        <v>0.71699999999999997</v>
       </c>
     </row>
     <row r="18" spans="1:10">
@@ -1093,37 +1102,66 @@
         <v>4</v>
       </c>
       <c r="D18" t="s">
+        <v>30</v>
+      </c>
+      <c r="E18">
+        <v>9605</v>
+      </c>
+      <c r="F18" t="s">
+        <v>31</v>
+      </c>
+      <c r="G18" t="s">
+        <v>10</v>
+      </c>
+      <c r="H18">
+        <v>0</v>
+      </c>
+      <c r="I18">
+        <v>0.248</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10">
+      <c r="A19">
+        <v>18</v>
+      </c>
+      <c r="B19" t="s">
+        <v>56</v>
+      </c>
+      <c r="C19">
+        <v>4</v>
+      </c>
+      <c r="D19" t="s">
         <v>32</v>
       </c>
-      <c r="E18">
+      <c r="E19">
         <v>4800</v>
       </c>
-      <c r="F18" t="s">
+      <c r="F19" t="s">
         <v>33</v>
       </c>
-      <c r="G18" t="s">
-        <v>10</v>
-      </c>
-      <c r="H18">
-        <v>0</v>
-      </c>
-      <c r="I18">
+      <c r="G19" t="s">
+        <v>10</v>
+      </c>
+      <c r="H19">
+        <v>0</v>
+      </c>
+      <c r="I19">
         <v>0.61499999999999999</v>
       </c>
     </row>
-    <row r="19" spans="1:10">
-      <c r="I19" t="s">
+    <row r="20" spans="1:10">
+      <c r="I20" t="s">
         <v>36</v>
       </c>
-      <c r="J19">
-        <f>SUM(I2:I18)</f>
-        <v>77.068999999999988</v>
+      <c r="J20">
+        <f>SUM(I2:I19)</f>
+        <v>83.23899999999999</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <ignoredErrors>
-    <ignoredError sqref="J12:J13" formulaRange="1"/>
+    <ignoredError sqref="J13:J14" formulaRange="1"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>